<commit_message>
Added promo-price to rozetka converter
</commit_message>
<xml_diff>
--- a/assets/rozetka_excel_example.xlsx
+++ b/assets/rozetka_excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Товары" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">Артикул</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">Розничная цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Промо цена</t>
   </si>
   <si>
     <t xml:space="preserve">Наличие (+ або -)</t>
@@ -530,42 +533,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BH8"/>
+  <dimension ref="A1:BI8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.0607287449393"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="27" min="17" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="33" min="29" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="37" min="36" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="44" min="39" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="56" min="46" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="60" min="58" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="61" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="17.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="17" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="29" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="24.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="39" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="46" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="58" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="61" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +602,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -745,6 +748,9 @@
       </c>
       <c r="BH1" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="48.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -752,7 +758,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -767,22 +773,23 @@
   </sheetPr>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,7 +821,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,7 +829,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +845,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,7 +861,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +877,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +893,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +909,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +917,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,7 +925,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +933,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +941,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +949,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +957,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,7 +965,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +973,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +981,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +989,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,7 +997,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,7 +1005,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,7 +1013,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,7 +1029,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1037,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1045,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1053,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +1061,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1069,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1077,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,7 +1085,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1093,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1101,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,13 +1109,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>